<commit_message>
Attempted a few combinations to see what would work best. So far HOG2 LDA1 SVM is one of the best combinations.
</commit_message>
<xml_diff>
--- a/Code/Saved/AllTrials.xlsx
+++ b/Code/Saved/AllTrials.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Repos\EmotionComparison\Code\Saved\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -76,16 +71,22 @@
   </si>
   <si>
     <t>SVM1</t>
+  </si>
+  <si>
+    <t>SVM4</t>
+  </si>
+  <si>
+    <t>SVM5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,13 +96,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,45 +135,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -226,7 +196,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -258,10 +228,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -293,7 +262,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -469,70 +437,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="8"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" ht="123" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:14">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="5">
-        <v>43416.659047777779</v>
+      <c r="B2" s="2">
+        <v>43416.65904777778</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -546,37 +504,37 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="8">
-        <v>0.69483568075117375</v>
-      </c>
-      <c r="H2" s="6">
-        <v>9.7017068862915039</v>
-      </c>
-      <c r="I2" s="6">
-        <v>9.1707229614257813</v>
-      </c>
-      <c r="J2" s="6">
-        <v>0.35598993301391602</v>
-      </c>
-      <c r="K2" s="6">
+      <c r="G2">
+        <v>0.6948356807511737</v>
+      </c>
+      <c r="H2">
+        <v>9.701706886291504</v>
+      </c>
+      <c r="I2">
+        <v>9.170722961425781</v>
+      </c>
+      <c r="J2">
+        <v>0.355989933013916</v>
+      </c>
+      <c r="K2">
         <v>0.1589851379394531</v>
       </c>
-      <c r="L2" s="6">
-        <v>1.419894695281982E-2</v>
-      </c>
-      <c r="M2" s="6">
-        <v>9.9971294403076181E-4</v>
-      </c>
-      <c r="N2" s="6">
-        <v>1.9991397857666021E-4</v>
+      <c r="L2">
+        <v>0.01419894695281982</v>
+      </c>
+      <c r="M2">
+        <v>0.0009997129440307618</v>
+      </c>
+      <c r="N2">
+        <v>0.0001999139785766602</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
-        <v>43416.659684629631</v>
+      <c r="B3" s="2">
+        <v>43416.65968462963</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -590,37 +548,37 @@
       <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="8">
-        <v>0.80281690140845074</v>
-      </c>
-      <c r="H3" s="6">
+      <c r="G3">
+        <v>0.8028169014084507</v>
+      </c>
+      <c r="H3">
         <v>22.90660452842712</v>
       </c>
-      <c r="I3" s="6">
-        <v>8.9697291851043701</v>
-      </c>
-      <c r="J3" s="6">
-        <v>1.7379386425018311</v>
-      </c>
-      <c r="K3" s="6">
-        <v>12.078939914703369</v>
-      </c>
-      <c r="L3" s="6">
-        <v>1.1671943426132201</v>
-      </c>
-      <c r="M3" s="6">
-        <v>1.8996477127075191E-3</v>
-      </c>
-      <c r="N3" s="6">
+      <c r="I3">
+        <v>8.96972918510437</v>
+      </c>
+      <c r="J3">
+        <v>1.737938642501831</v>
+      </c>
+      <c r="K3">
+        <v>12.07893991470337</v>
+      </c>
+      <c r="L3">
+        <v>1.16719434261322</v>
+      </c>
+      <c r="M3">
+        <v>0.001899647712707519</v>
+      </c>
+      <c r="N3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
-        <v>43416.660201440012</v>
+      <c r="B4" s="2">
+        <v>43416.66020143519</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -634,29 +592,249 @@
       <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="8">
-        <v>0.16901408450704231</v>
-      </c>
-      <c r="H4" s="6">
-        <v>21.758917808532711</v>
-      </c>
-      <c r="I4" s="6">
-        <v>9.4327163696289063</v>
-      </c>
-      <c r="J4" s="6">
+      <c r="G4">
+        <v>0.1690140845070423</v>
+      </c>
+      <c r="H4">
+        <v>21.75891780853271</v>
+      </c>
+      <c r="I4">
+        <v>9.432716369628906</v>
+      </c>
+      <c r="J4">
         <v>1.84895396232605</v>
       </c>
-      <c r="K4" s="6">
-        <v>10.336251735687259</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0.97312762737274172</v>
-      </c>
-      <c r="M4" s="6">
-        <v>1.7899560928344729E-2</v>
-      </c>
-      <c r="N4" s="6">
-        <v>1.099824905395508E-3</v>
+      <c r="K4">
+        <v>10.33625173568726</v>
+      </c>
+      <c r="L4">
+        <v>0.9731276273727417</v>
+      </c>
+      <c r="M4">
+        <v>0.01789956092834473</v>
+      </c>
+      <c r="N4">
+        <v>0.001099824905395508</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43416.83220528935</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5">
+        <v>0.8028169014084507</v>
+      </c>
+      <c r="H5">
+        <v>25.91721534729004</v>
+      </c>
+      <c r="I5">
+        <v>9.262726068496704</v>
+      </c>
+      <c r="J5">
+        <v>1.78394603729248</v>
+      </c>
+      <c r="K5">
+        <v>14.73854637145996</v>
+      </c>
+      <c r="L5">
+        <v>1.425658130645752</v>
+      </c>
+      <c r="M5">
+        <v>0.001999378204345703</v>
+      </c>
+      <c r="N5">
+        <v>0.00019989013671875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>43416.83263604167</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <v>0.8075117370892019</v>
+      </c>
+      <c r="H6">
+        <v>27.80616283416748</v>
+      </c>
+      <c r="I6">
+        <v>9.993708610534668</v>
+      </c>
+      <c r="J6">
+        <v>2.283921003341675</v>
+      </c>
+      <c r="K6">
+        <v>15.39253664016724</v>
+      </c>
+      <c r="L6">
+        <v>1.488454985618591</v>
+      </c>
+      <c r="M6">
+        <v>0.002599716186523438</v>
+      </c>
+      <c r="N6">
+        <v>9.996891021728516e-05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43416.83310738426</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>0.8075117370892019</v>
+      </c>
+      <c r="H7">
+        <v>28.5735125541687</v>
+      </c>
+      <c r="I7">
+        <v>10.25267958641052</v>
+      </c>
+      <c r="J7">
+        <v>2.362849473953247</v>
+      </c>
+      <c r="K7">
+        <v>15.81077837944031</v>
+      </c>
+      <c r="L7">
+        <v>1.52377815246582</v>
+      </c>
+      <c r="M7">
+        <v>0.007899713516235352</v>
+      </c>
+      <c r="N7">
+        <v>0.0002998828887939453</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>43416.83585619213</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8">
+        <v>0.6901408450704225</v>
+      </c>
+      <c r="H8">
+        <v>9.813695669174194</v>
+      </c>
+      <c r="I8">
+        <v>9.25572657585144</v>
+      </c>
+      <c r="J8">
+        <v>0.3749740123748779</v>
+      </c>
+      <c r="K8">
+        <v>0.1599812507629395</v>
+      </c>
+      <c r="L8">
+        <v>0.01429970264434815</v>
+      </c>
+      <c r="M8">
+        <v>0.000998544692993164</v>
+      </c>
+      <c r="N8">
+        <v>9.989738464355469e-05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>43416.83613629657</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9">
+        <v>0.6948356807511737</v>
+      </c>
+      <c r="H9">
+        <v>10.26790833473206</v>
+      </c>
+      <c r="I9">
+        <v>9.718909025192261</v>
+      </c>
+      <c r="J9">
+        <v>0.3650102615356445</v>
+      </c>
+      <c r="K9">
+        <v>0.1679892539978027</v>
+      </c>
+      <c r="L9">
+        <v>0.01480016708374023</v>
+      </c>
+      <c r="M9">
+        <v>0.0009995222091674805</v>
+      </c>
+      <c r="N9">
+        <v>9.996891021728516e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got LBP working with LBP8 and SVM2 at >80%
</commit_message>
<xml_diff>
--- a/Code/Saved/AllTrials.xlsx
+++ b/Code/Saved/AllTrials.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -64,6 +64,45 @@
     <t>HOG2</t>
   </si>
   <si>
+    <t>LBP1</t>
+  </si>
+  <si>
+    <t>LBP2</t>
+  </si>
+  <si>
+    <t>LBP3</t>
+  </si>
+  <si>
+    <t>LBP4</t>
+  </si>
+  <si>
+    <t>LBP5</t>
+  </si>
+  <si>
+    <t>LBP6</t>
+  </si>
+  <si>
+    <t>LBP7</t>
+  </si>
+  <si>
+    <t>LBP8</t>
+  </si>
+  <si>
+    <t>LBP9</t>
+  </si>
+  <si>
+    <t>LBP10</t>
+  </si>
+  <si>
+    <t>LBP11</t>
+  </si>
+  <si>
+    <t>LBP12</t>
+  </si>
+  <si>
+    <t>LBP13</t>
+  </si>
+  <si>
     <t>LDA1</t>
   </si>
   <si>
@@ -77,6 +116,15 @@
   </si>
   <si>
     <t>SVM5</t>
+  </si>
+  <si>
+    <t>SVM6</t>
+  </si>
+  <si>
+    <t>SVM2</t>
+  </si>
+  <si>
+    <t>SVM3</t>
   </si>
 </sst>
 </file>
@@ -438,7 +486,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -499,10 +547,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G2">
         <v>0.6948356807511737</v>
@@ -543,10 +591,10 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G3">
         <v>0.8028169014084507</v>
@@ -587,10 +635,10 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G4">
         <v>0.1690140845070423</v>
@@ -631,10 +679,10 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G5">
         <v>0.8028169014084507</v>
@@ -675,10 +723,10 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G6">
         <v>0.8075117370892019</v>
@@ -719,10 +767,10 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G7">
         <v>0.8075117370892019</v>
@@ -763,10 +811,10 @@
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G8">
         <v>0.6901408450704225</v>
@@ -798,7 +846,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>43416.83613629657</v>
+        <v>43416.8361362963</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -807,10 +855,10 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G9">
         <v>0.6948356807511737</v>
@@ -835,6 +883,923 @@
       </c>
       <c r="N9">
         <v>9.996891021728516e-05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>43417.90567797454</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10">
+        <v>0.6948356807511737</v>
+      </c>
+      <c r="H10">
+        <v>13.89690470695496</v>
+      </c>
+      <c r="I10">
+        <v>9.036727905273438</v>
+      </c>
+      <c r="J10">
+        <v>0.4019877910614014</v>
+      </c>
+      <c r="K10">
+        <v>4.387868165969849</v>
+      </c>
+      <c r="L10">
+        <v>0.4226877212524414</v>
+      </c>
+      <c r="M10">
+        <v>0.001799464225769043</v>
+      </c>
+      <c r="N10">
+        <v>9.996891021728516e-05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>43417.90944876157</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11">
+        <v>0.3286384976525822</v>
+      </c>
+      <c r="H11">
+        <v>9.51680850982666</v>
+      </c>
+      <c r="I11">
+        <v>8.994744062423706</v>
+      </c>
+      <c r="J11">
+        <v>0.4609818458557129</v>
+      </c>
+      <c r="K11">
+        <v>0.03604769706726074</v>
+      </c>
+      <c r="L11">
+        <v>0.001300716400146484</v>
+      </c>
+      <c r="M11">
+        <v>0.001703071594238281</v>
+      </c>
+      <c r="N11">
+        <v>0.0003000020980834961</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>43417.91138012731</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12">
+        <v>0.2206572769953052</v>
+      </c>
+      <c r="H12">
+        <v>9.55771279335022</v>
+      </c>
+      <c r="I12">
+        <v>9.011727571487427</v>
+      </c>
+      <c r="J12">
+        <v>0.4999716281890869</v>
+      </c>
+      <c r="K12">
+        <v>0.03301382064819336</v>
+      </c>
+      <c r="L12">
+        <v>0.001198267936706543</v>
+      </c>
+      <c r="M12">
+        <v>0.001500177383422852</v>
+      </c>
+      <c r="N12">
+        <v>0.0002014875411987305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>43417.91161951389</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13">
+        <v>0.2206572769953052</v>
+      </c>
+      <c r="H13">
+        <v>9.496700048446655</v>
+      </c>
+      <c r="I13">
+        <v>8.978724718093872</v>
+      </c>
+      <c r="J13">
+        <v>0.4729859828948975</v>
+      </c>
+      <c r="K13">
+        <v>0.03198933601379395</v>
+      </c>
+      <c r="L13">
+        <v>0.0009989976882934571</v>
+      </c>
+      <c r="M13">
+        <v>0.001600027084350586</v>
+      </c>
+      <c r="N13">
+        <v>9.999275207519531e-05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>43417.9130608912</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14">
+        <v>0.1408450704225352</v>
+      </c>
+      <c r="H14">
+        <v>33.39202427864075</v>
+      </c>
+      <c r="I14">
+        <v>8.991738557815552</v>
+      </c>
+      <c r="J14">
+        <v>2.452926158905029</v>
+      </c>
+      <c r="K14">
+        <v>21.75434565544128</v>
+      </c>
+      <c r="L14">
+        <v>2.109036111831665</v>
+      </c>
+      <c r="M14">
+        <v>0.002500081062316895</v>
+      </c>
+      <c r="N14">
+        <v>0.0002000570297241211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>43417.91455135417</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15">
+        <v>0.2018779342723005</v>
+      </c>
+      <c r="H15">
+        <v>59.39724493026733</v>
+      </c>
+      <c r="I15">
+        <v>9.06171727180481</v>
+      </c>
+      <c r="J15">
+        <v>2.371943950653076</v>
+      </c>
+      <c r="K15">
+        <v>47.750572681427</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>4.464963054656982</v>
+      </c>
+      <c r="N15">
+        <v>0.2504944086074829</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>43417.91558442129</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16">
+        <v>0.3145539906103286</v>
+      </c>
+      <c r="H16">
+        <v>11.68264818191528</v>
+      </c>
+      <c r="I16">
+        <v>9.492714166641235</v>
+      </c>
+      <c r="J16">
+        <v>2.131935834884644</v>
+      </c>
+      <c r="K16">
+        <v>0.03199887275695801</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0.00279996395111084</v>
+      </c>
+      <c r="N16">
+        <v>9.992122650146485e-05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>43417.91769465278</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17">
+        <v>0.3145539906103286</v>
+      </c>
+      <c r="H17">
+        <v>11.62885165214539</v>
+      </c>
+      <c r="I17">
+        <v>9.268705129623413</v>
+      </c>
+      <c r="J17">
+        <v>2.304138660430908</v>
+      </c>
+      <c r="K17">
+        <v>0.04100751876831055</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0.003498339653015137</v>
+      </c>
+      <c r="N17">
+        <v>0.0002009868621826172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <v>43417.92074293982</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18">
+        <v>0.3145539906103286</v>
+      </c>
+      <c r="H18">
+        <v>11.31365942955017</v>
+      </c>
+      <c r="I18">
+        <v>9.126725196838379</v>
+      </c>
+      <c r="J18">
+        <v>2.13993501663208</v>
+      </c>
+      <c r="K18">
+        <v>0.03299856185913086</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0.002698969841003418</v>
+      </c>
+      <c r="N18">
+        <v>0.0002008438110351562</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2">
+        <v>43417.92231515046</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19">
+        <v>0.3286384976525822</v>
+      </c>
+      <c r="H19">
+        <v>15.25253319740295</v>
+      </c>
+      <c r="I19">
+        <v>9.080719232559204</v>
+      </c>
+      <c r="J19">
+        <v>2.144947052001953</v>
+      </c>
+      <c r="K19">
+        <v>4.013878583908081</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0.4008879423141479</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <v>43417.92302503472</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20">
+        <v>0.4084507042253521</v>
+      </c>
+      <c r="H20">
+        <v>12.9866042137146</v>
+      </c>
+      <c r="I20">
+        <v>9.194708347320557</v>
+      </c>
+      <c r="J20">
+        <v>3.124915838241577</v>
+      </c>
+      <c r="K20">
+        <v>0.6539897918701172</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0.06469745635986328</v>
+      </c>
+      <c r="N20">
+        <v>0.0004000663757324219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2">
+        <v>43417.92364842592</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21">
+        <v>0.5023474178403756</v>
+      </c>
+      <c r="H21">
+        <v>15.42652869224548</v>
+      </c>
+      <c r="I21">
+        <v>9.192713975906372</v>
+      </c>
+      <c r="J21">
+        <v>6.152823686599731</v>
+      </c>
+      <c r="K21">
+        <v>0.06799077987670898</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0.00609886646270752</v>
+      </c>
+      <c r="N21">
+        <v>0.0003000497817993164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2">
+        <v>43417.92416144676</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22">
+        <v>0.5023474178403756</v>
+      </c>
+      <c r="H22">
+        <v>15.4135365486145</v>
+      </c>
+      <c r="I22">
+        <v>9.119731187820435</v>
+      </c>
+      <c r="J22">
+        <v>6.212807655334473</v>
+      </c>
+      <c r="K22">
+        <v>0.06599783897399902</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0.005999779701232911</v>
+      </c>
+      <c r="N22">
+        <v>0.0003000020980834961</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2">
+        <v>43417.92457196759</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23">
+        <v>0.6572769953051644</v>
+      </c>
+      <c r="H23">
+        <v>18.11044049263</v>
+      </c>
+      <c r="I23">
+        <v>9.123711109161377</v>
+      </c>
+      <c r="J23">
+        <v>8.904741764068604</v>
+      </c>
+      <c r="K23">
+        <v>0.06598758697509766</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0.005899786949157715</v>
+      </c>
+      <c r="N23">
+        <v>0.0002999782562255859</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2">
+        <v>43417.92526445602</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24">
+        <v>0.3943661971830986</v>
+      </c>
+      <c r="H24">
+        <v>21.57535028457642</v>
+      </c>
+      <c r="I24">
+        <v>9.099725246429443</v>
+      </c>
+      <c r="J24">
+        <v>12.3626389503479</v>
+      </c>
+      <c r="K24">
+        <v>0.09698700904846191</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0.008898687362670899</v>
+      </c>
+      <c r="N24">
+        <v>0.0003999948501586914</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2">
+        <v>43417.92637712963</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25">
+        <v>0.5539906103286385</v>
+      </c>
+      <c r="H25">
+        <v>20.94436001777649</v>
+      </c>
+      <c r="I25">
+        <v>9.168729305267334</v>
+      </c>
+      <c r="J25">
+        <v>11.67363405227661</v>
+      </c>
+      <c r="K25">
+        <v>0.08899664878845215</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0.008098983764648437</v>
+      </c>
+      <c r="N25">
+        <v>0.0003006219863891602</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2">
+        <v>43417.9271562963</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26">
+        <v>0.5023474178403756</v>
+      </c>
+      <c r="H26">
+        <v>26.4082145690918</v>
+      </c>
+      <c r="I26">
+        <v>9.119734525680542</v>
+      </c>
+      <c r="J26">
+        <v>17.15647387504578</v>
+      </c>
+      <c r="K26">
+        <v>0.1179964542388916</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0.01089730262756348</v>
+      </c>
+      <c r="N26">
+        <v>0.0005024433135986328</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2">
+        <v>43417.92785108796</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27">
+        <v>0.5633802816901409</v>
+      </c>
+      <c r="H27">
+        <v>21.3263726234436</v>
+      </c>
+      <c r="I27">
+        <v>9.188733577728271</v>
+      </c>
+      <c r="J27">
+        <v>12.04162764549255</v>
+      </c>
+      <c r="K27">
+        <v>0.08201193809509277</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0.007501363754272461</v>
+      </c>
+      <c r="N27">
+        <v>0.0002999305725097656</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2">
+        <v>43417.9295352199</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28">
+        <v>0.6572769953051644</v>
+      </c>
+      <c r="H28">
+        <v>21.54404973983765</v>
+      </c>
+      <c r="I28">
+        <v>11.31635737419128</v>
+      </c>
+      <c r="J28">
+        <v>10.14868521690369</v>
+      </c>
+      <c r="K28">
+        <v>0.06500649452209473</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0.00590057373046875</v>
+      </c>
+      <c r="N28">
+        <v>0.0002992391586303711</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2">
+        <v>43417.93019828704</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29">
+        <v>0.2629107981220657</v>
+      </c>
+      <c r="H29">
+        <v>18.23745131492615</v>
+      </c>
+      <c r="I29">
+        <v>9.096725940704346</v>
+      </c>
+      <c r="J29">
+        <v>9.042729377746582</v>
+      </c>
+      <c r="K29">
+        <v>0.08399748802185059</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0.007499814033508301</v>
+      </c>
+      <c r="N29">
+        <v>0.0002000093460083008</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2">
+        <v>43417.93067200232</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30">
+        <v>0.8169014084507042</v>
+      </c>
+      <c r="H30">
+        <v>18.19046330451965</v>
+      </c>
+      <c r="I30">
+        <v>9.10072660446167</v>
+      </c>
+      <c r="J30">
+        <v>8.990729808807373</v>
+      </c>
+      <c r="K30">
+        <v>0.08600640296936035</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0.007999277114868164</v>
+      </c>
+      <c r="N30">
+        <v>0.0003000020980834961</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2">
+        <v>43417.93120255879</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31">
+        <v>0.7370892018779343</v>
+      </c>
+      <c r="H31">
+        <v>18.16645336151123</v>
+      </c>
+      <c r="I31">
+        <v>9.071726560592651</v>
+      </c>
+      <c r="J31">
+        <v>9.009729623794556</v>
+      </c>
+      <c r="K31">
+        <v>0.06999731063842773</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0.00629875659942627</v>
+      </c>
+      <c r="N31">
+        <v>0.0003010034561157227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Attempted feature selection/reduction techniques with no luck
</commit_message>
<xml_diff>
--- a/Code/Saved/AllTrials.xlsx
+++ b/Code/Saved/AllTrials.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -486,7 +486,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1766,7 +1766,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="2">
-        <v>43417.93120255879</v>
+        <v>43417.93120255787</v>
       </c>
       <c r="C31" t="s">
         <v>13</v>
@@ -1800,6 +1800,314 @@
       </c>
       <c r="N31">
         <v>0.0003010034561157227</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2">
+        <v>43417.93338178241</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32">
+        <v>0.4553990610328639</v>
+      </c>
+      <c r="H32">
+        <v>18.10745525360107</v>
+      </c>
+      <c r="I32">
+        <v>9.070727109909058</v>
+      </c>
+      <c r="J32">
+        <v>8.942731380462646</v>
+      </c>
+      <c r="K32">
+        <v>0.07999753952026367</v>
+      </c>
+      <c r="L32">
+        <v>0.005600118637084961</v>
+      </c>
+      <c r="M32">
+        <v>0.001500535011291504</v>
+      </c>
+      <c r="N32">
+        <v>0.0003999948501586914</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2">
+        <v>43417.93377541667</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33">
+        <v>0.4647887323943662</v>
+      </c>
+      <c r="H33">
+        <v>18.38443160057068</v>
+      </c>
+      <c r="I33">
+        <v>9.267715930938721</v>
+      </c>
+      <c r="J33">
+        <v>8.999729156494141</v>
+      </c>
+      <c r="K33">
+        <v>0.1039659976959229</v>
+      </c>
+      <c r="L33">
+        <v>0.002099084854125977</v>
+      </c>
+      <c r="M33">
+        <v>0.007399535179138184</v>
+      </c>
+      <c r="N33">
+        <v>0.0005000114440917968</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2">
+        <v>43417.93413646991</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34">
+        <v>0.5070422535211268</v>
+      </c>
+      <c r="H34">
+        <v>18.65042853355408</v>
+      </c>
+      <c r="I34">
+        <v>9.126715183258057</v>
+      </c>
+      <c r="J34">
+        <v>9.463715076446533</v>
+      </c>
+      <c r="K34">
+        <v>0.04698753356933594</v>
+      </c>
+      <c r="L34">
+        <v>0.003199863433837891</v>
+      </c>
+      <c r="M34">
+        <v>0.001100015640258789</v>
+      </c>
+      <c r="N34">
+        <v>9.9945068359375e-05</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2">
+        <v>43417.93451767361</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35">
+        <v>0.3051643192488263</v>
+      </c>
+      <c r="H35">
+        <v>18.46443343162537</v>
+      </c>
+      <c r="I35">
+        <v>9.061725616455078</v>
+      </c>
+      <c r="J35">
+        <v>9.333709955215454</v>
+      </c>
+      <c r="K35">
+        <v>0.05399847030639648</v>
+      </c>
+      <c r="L35">
+        <v>0.003000235557556152</v>
+      </c>
+      <c r="M35">
+        <v>0.001799774169921875</v>
+      </c>
+      <c r="N35">
+        <v>0.0001999139785766602</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2">
+        <v>43417.93495306713</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36">
+        <v>0.5539906103286385</v>
+      </c>
+      <c r="H36">
+        <v>18.37643694877625</v>
+      </c>
+      <c r="I36">
+        <v>9.139714479446411</v>
+      </c>
+      <c r="J36">
+        <v>9.133739709854126</v>
+      </c>
+      <c r="K36">
+        <v>0.08898758888244629</v>
+      </c>
+      <c r="L36">
+        <v>0.001899242401123047</v>
+      </c>
+      <c r="M36">
+        <v>0.006199479103088379</v>
+      </c>
+      <c r="N36">
+        <v>0.0005001068115234375</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2">
+        <v>43417.93529873843</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37">
+        <v>0.4694835680751174</v>
+      </c>
+      <c r="H37">
+        <v>18.76842522621155</v>
+      </c>
+      <c r="I37">
+        <v>9.079715728759766</v>
+      </c>
+      <c r="J37">
+        <v>9.563712596893311</v>
+      </c>
+      <c r="K37">
+        <v>0.1119873523712158</v>
+      </c>
+      <c r="L37">
+        <v>0.002299070358276367</v>
+      </c>
+      <c r="M37">
+        <v>0.008099508285522462</v>
+      </c>
+      <c r="N37">
+        <v>0.0004001379013061523</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2">
+        <v>43417.93577364587</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" t="s">
+        <v>35</v>
+      </c>
+      <c r="G38">
+        <v>0.4647887323943662</v>
+      </c>
+      <c r="H38">
+        <v>18.54843211174011</v>
+      </c>
+      <c r="I38">
+        <v>9.096726894378662</v>
+      </c>
+      <c r="J38">
+        <v>9.32970929145813</v>
+      </c>
+      <c r="K38">
+        <v>0.1079964637756348</v>
+      </c>
+      <c r="L38">
+        <v>0.001898932456970215</v>
+      </c>
+      <c r="M38">
+        <v>0.007799482345581055</v>
+      </c>
+      <c r="N38">
+        <v>0.0006002426147460937</v>
       </c>
     </row>
   </sheetData>

</xml_diff>